<commit_message>
added CAGR support added from df support
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25703"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26207"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schien/workspaces/python/guardian2015/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schien/workspaces/python/excel-modeling-tools/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>variable</t>
   </si>
@@ -108,6 +108,33 @@
   </si>
   <si>
     <t>s1</t>
+  </si>
+  <si>
+    <t>start date</t>
+  </si>
+  <si>
+    <t>end date</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>ref date</t>
+  </si>
+  <si>
+    <t>CAGR</t>
+  </si>
+  <si>
+    <t>multiple choice</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
   </si>
 </sst>
 </file>
@@ -171,7 +198,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -179,19 +206,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -526,18 +559,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -562,11 +596,29 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
         <v>7</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -579,12 +631,26 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="3">
+        <v>39814</v>
+      </c>
+      <c r="J2" s="3">
+        <v>39904</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="L2" s="3">
+        <v>39814</v>
+      </c>
+      <c r="M2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -604,11 +670,11 @@
       <c r="H3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -630,11 +696,11 @@
       <c r="H4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -652,11 +718,11 @@
       <c r="H5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -673,7 +739,35 @@
         <v>2</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" t="s">
+      <c r="M7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="3">
+        <v>39083</v>
+      </c>
+      <c r="J8" s="3">
+        <v>39814</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
catch non-initialised item access to prepare item for access
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schien/workspaces/python/excel-modeling-tools/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/python/excel-modeling-tools/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
   <si>
     <t>variable</t>
   </si>
@@ -75,15 +75,9 @@
     <t>-</t>
   </si>
   <si>
-    <t>core overcapacity</t>
-  </si>
-  <si>
     <t>triangular</t>
   </si>
   <si>
-    <t>number core hops</t>
-  </si>
-  <si>
     <t>bottom_up_comparision.sampling_core_routers</t>
   </si>
   <si>
@@ -94,9 +88,6 @@
   </si>
   <si>
     <t>J/Gb</t>
-  </si>
-  <si>
-    <t>core router efficiency</t>
   </si>
   <si>
     <t>b</t>
@@ -565,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,25 +592,25 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M1" t="s">
         <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -636,7 +627,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I2" s="3">
         <v>39814</v>
@@ -656,7 +647,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -675,18 +666,18 @@
         <v>14</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
@@ -701,29 +692,29 @@
         <v>14</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -731,7 +722,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -749,7 +740,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -758,10 +749,10 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I8" s="3">
         <v>39083</v>
@@ -785,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -817,30 +808,30 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M1" t="s">
         <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -852,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I2" s="3">
         <v>39814</v>

</xml_diff>

<commit_message>
added excel data source reload now python 3 only
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,38 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/python/excel-modeling-tools/tests/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-  </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$2</definedName>
-  </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr codeName="ThisWorkbook"/>
+  <s:bookViews>
+    <s:workbookView activeTab="0"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <s:sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>variable</t>
   </si>
   <si>
+    <t>scenario</t>
+  </si>
+  <si>
     <t>module</t>
   </si>
   <si>
@@ -51,10 +41,25 @@
     <t>unit</t>
   </si>
   <si>
+    <t>start date</t>
+  </si>
+  <si>
+    <t>end date</t>
+  </si>
+  <si>
+    <t>CAGR</t>
+  </si>
+  <si>
+    <t>ref date</t>
+  </si>
+  <si>
     <t>label</t>
   </si>
   <si>
-    <t>scenario</t>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>source</t>
   </si>
   <si>
     <t>a</t>
@@ -66,18 +71,30 @@
     <t>choice</t>
   </si>
   <si>
+    <t>kg</t>
+  </si>
+  <si>
     <t>test var 1</t>
   </si>
   <si>
+    <t>b</t>
+  </si>
+  <si>
     <t>uniform</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
+    <t>c</t>
+  </si>
+  <si>
     <t>triangular</t>
   </si>
   <si>
+    <t>d</t>
+  </si>
+  <si>
     <t>bottom_up_comparision.sampling_core_routers</t>
   </si>
   <si>
@@ -90,37 +107,7 @@
     <t>J/Gb</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
     <t>s1</t>
-  </si>
-  <si>
-    <t>start date</t>
-  </si>
-  <si>
-    <t>end date</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>kg</t>
-  </si>
-  <si>
-    <t>ref date</t>
-  </si>
-  <si>
-    <t>CAGR</t>
   </si>
   <si>
     <t>multiple choice</t>
@@ -135,50 +122,35 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
       <sz val="12"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -193,42 +165,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -553,315 +504,321 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:sheetPr>
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+  </s:sheetPr>
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="13.5"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="40.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>27</v>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>39814</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>39904</v>
+      </c>
+      <c r="K2" s="4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>39814</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="3">
-        <v>39814</v>
-      </c>
-      <c r="J2" s="3">
-        <v>39904</v>
-      </c>
-      <c r="K2" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="L2" s="3">
-        <v>39814</v>
-      </c>
-      <c r="M2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="n"/>
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="2" t="n"/>
+      <c r="G5" s="1" t="n"/>
+      <c r="H5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="1">
-        <v>4</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>7</v>
+      <c r="H7" s="1" t="n"/>
+      <c r="M7" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1">
-        <v>6</v>
-      </c>
-      <c r="G4" s="1">
-        <v>10</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="M7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
         <v>32</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="3">
+        <v>18</v>
+      </c>
+      <c r="I8" s="3" t="n">
         <v>39083</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="3" t="n">
         <v>39814</v>
       </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="K8" s="3" t="n"/>
+      <c r="L8" s="3" t="n"/>
       <c r="M8" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <s:pageSetup horizontalDpi="4294967292" orientation="portrait" paperSize="9" verticalDpi="4294967292"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:sheetPr>
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+  </s:sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2">
+        <v>17</v>
+      </c>
+      <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="3">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="n">
         <v>39814</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="3" t="n">
         <v>39904</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="3" t="n">
         <v>39814</v>
       </c>
       <c r="M2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added python 2.7 support back in
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -504,10 +504,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -722,15 +723,16 @@
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <s:pageSetup horizontalDpi="4294967292" orientation="portrait" paperSize="9" verticalDpi="4294967292"/>
+  <pageSetup horizontalDpi="4294967292" orientation="portrait" paperSize="9" verticalDpi="4294967292"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
added test fixed install dependencies
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr codeName="ThisWorkbook"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <s:sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/python/excel-modeling-tools/tests/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="540" windowWidth="28560" windowHeight="17380"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+  </sheets>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
   <si>
     <t>variable</t>
   </si>
@@ -117,40 +127,45 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>minutes/month</t>
+  </si>
+  <si>
+    <t>mm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -166,20 +181,26 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -504,24 +525,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-    <s:pageSetUpPr/>
-  </s:sheetPr>
-  <dimension ref="A1:O8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="13.5"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="40.6640625"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +585,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -578,29 +595,29 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="3">
         <v>39814</v>
       </c>
-      <c r="J2" s="3" t="n">
+      <c r="J2" s="3">
         <v>39904</v>
       </c>
-      <c r="K2" s="4" t="n">
+      <c r="K2" s="4">
         <v>0.1</v>
       </c>
-      <c r="L2" s="3" t="n">
+      <c r="L2" s="3">
         <v>39814</v>
       </c>
       <c r="M2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -610,13 +627,13 @@
       <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="1">
         <v>2</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="1">
         <v>4</v>
       </c>
-      <c r="G3" s="1" t="n"/>
+      <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
@@ -624,7 +641,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -634,13 +651,13 @@
       <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="1">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="1">
         <v>6</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="G4" s="1">
         <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -650,7 +667,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -663,8 +680,8 @@
       <c r="E5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="2" t="n"/>
-      <c r="G5" s="1" t="n"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
         <v>29</v>
       </c>
@@ -672,7 +689,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -685,15 +702,15 @@
       <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>2</v>
       </c>
-      <c r="H7" s="1" t="n"/>
+      <c r="H7" s="1"/>
       <c r="M7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -709,39 +726,66 @@
       <c r="H8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="3" t="n">
+      <c r="I8" s="3">
         <v>39083</v>
       </c>
-      <c r="J8" s="3" t="n">
+      <c r="J8" s="3">
         <v>39814</v>
       </c>
-      <c r="K8" s="3" t="n"/>
-      <c r="L8" s="3" t="n"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
       <c r="M8" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="5">
+        <f>6000000000*60</f>
+        <v>360000000000</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="H10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="3">
+        <v>42005</v>
+      </c>
+      <c r="J10" s="3">
+        <v>42370</v>
+      </c>
+      <c r="K10">
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="3">
+        <v>42005</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <s:pageSetup horizontalDpi="4294967292" orientation="portrait" paperSize="9" verticalDpi="4294967292"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-    <s:pageSetUpPr/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -788,7 +832,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -798,22 +842,22 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="3">
         <v>39814</v>
       </c>
-      <c r="J2" s="3" t="n">
+      <c r="J2" s="3">
         <v>39904</v>
       </c>
-      <c r="K2" s="4" t="n">
+      <c r="K2" s="4">
         <v>0.1</v>
       </c>
-      <c r="L2" s="3" t="n">
+      <c r="L2" s="3">
         <v>39814</v>
       </c>
       <c r="M2" t="s">
@@ -821,6 +865,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new flag 'single_var' to freeze all variables except one to their mean value - use in sensitivity analysis.
For variables without ref_date, start_date, end_date - use time index from Dataset
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -17,6 +17,9 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>variable</t>
   </si>
@@ -133,6 +136,12 @@
   </si>
   <si>
     <t>mm</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>normal</t>
   </si>
 </sst>
 </file>
@@ -529,7 +538,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -687,6 +696,24 @@
       </c>
       <c r="M5" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f>E6/10</f>
+        <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
proper test case for 'single_var' kwarg add xarray to dependencies inc to v 0.3.0
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,34 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/python/excel-modeling-tools/tests/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="540" windowWidth="28560" windowHeight="17380"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-  </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr codeName="ThisWorkbook"/>
+  <s:bookViews>
+    <s:workbookView activeTab="0"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <s:sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>variable</t>
   </si>
@@ -120,6 +107,12 @@
     <t>J/Gb</t>
   </si>
   <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
     <t>s1</t>
   </si>
   <si>
@@ -129,52 +122,47 @@
     <t>1,2,3</t>
   </si>
   <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>minutes/month</t>
+  </si>
+  <si>
     <t>z</t>
-  </si>
-  <si>
-    <t>minutes/month</t>
-  </si>
-  <si>
-    <t>mm</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>normal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -190,26 +178,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="11" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -534,20 +517,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="13.5"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="40.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -594,7 +581,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -604,29 +591,29 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="3" t="n">
         <v>39814</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="3" t="n">
         <v>39904</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="3" t="n">
         <v>39814</v>
       </c>
       <c r="M2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -636,13 +623,13 @@
       <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1" t="n"/>
       <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
@@ -650,7 +637,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -660,13 +647,13 @@
       <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="1" t="n">
         <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -676,7 +663,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -689,8 +676,8 @@
       <c r="E5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="1"/>
+      <c r="F5" s="2" t="n"/>
+      <c r="G5" s="1" t="n"/>
       <c r="H5" s="1" t="s">
         <v>29</v>
       </c>
@@ -698,30 +685,30 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6">
+        <v>31</v>
+      </c>
+      <c r="E6" t="n">
         <v>1</v>
       </c>
       <c r="F6">
         <f>E6/10</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -729,17 +716,17 @@
       <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>2</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1" t="n"/>
       <c r="M7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
@@ -748,24 +735,24 @@
         <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="3" t="n">
         <v>39083</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="3" t="n">
         <v>39814</v>
       </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="K8" s="3" t="n"/>
+      <c r="L8" s="3" t="n"/>
       <c r="M8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -775,44 +762,47 @@
       <c r="D10" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="5">
-        <f>6000000000*60</f>
-        <v>360000000000</v>
-      </c>
-      <c r="F10" s="5"/>
+      <c r="E10" s="5" t="n">
+        <v>123</v>
+      </c>
+      <c r="F10" s="5" t="n"/>
       <c r="H10" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="3">
+        <v>36</v>
+      </c>
+      <c r="I10" s="3" t="n">
         <v>42005</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="3" t="n">
         <v>42370</v>
       </c>
-      <c r="K10">
+      <c r="K10" t="n">
         <v>0.5</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="3" t="n">
         <v>42005</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="4294967292" orientation="portrait" paperSize="9" verticalDpi="4294967292"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -859,9 +849,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -869,22 +859,22 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="3" t="n">
         <v>39814</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="3" t="n">
         <v>39904</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="3" t="n">
         <v>39814</v>
       </c>
       <c r="M2" t="s">
@@ -892,6 +882,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added option to sample_mean_value from distributions
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="680" windowWidth="28560" windowHeight="17380"/>
+    <workbookView xWindow="240" yWindow="540" windowWidth="28560" windowHeight="17380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -580,7 +580,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -647,6 +647,7 @@
         <v>17</v>
       </c>
       <c r="E2">
+        <f>E3/F$2</f>
         <v>1</v>
       </c>
       <c r="F2">

</xml_diff>

<commit_message>
fix random function initialisation: ignore None and empty strings
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/python/excel-modeling-tools/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3140D8D-104A-844E-9037-50D6B595BB12}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="3240" windowWidth="28560" windowHeight="17380" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="620" windowWidth="28560" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="44">
   <si>
     <t>variable</t>
   </si>
@@ -154,12 +155,18 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>static_one</t>
+  </si>
+  <si>
+    <t>litres</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -247,6 +254,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -573,11 +583,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -949,7 +959,36 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
+      <c r="A14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="3">
+        <v>39814</v>
+      </c>
+      <c r="J14" s="3">
+        <v>39904</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="L14" s="3">
+        <v>39814</v>
+      </c>
+      <c r="M14" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -958,10 +997,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- refactoring: store simulation results in subfolder output/model name / datetime - server: new page compare_runs/model name to compare model runs
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/python/excel-modeling-tools/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/python/excel-modelling-tools/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3140D8D-104A-844E-9037-50D6B595BB12}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1024D9-63FA-6243-87B5-254D422E1436}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="620" windowWidth="28560" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9840" yWindow="4220" windowWidth="28560" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -587,7 +587,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:M14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>